<commit_message>
certificate with places are added
</commit_message>
<xml_diff>
--- a/assets/assets/certificate.xlsx
+++ b/assets/assets/certificate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="183">
   <si>
     <t>SI</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Al Ameen </t>
     </r>
     <r>
@@ -250,6 +256,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">S4 </t>
     </r>
     <r>
@@ -502,18 +514,140 @@
   <si>
     <t>Beneeta</t>
   </si>
+  <si>
+    <t>FIRST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARATH SANTHOSH </t>
+  </si>
+  <si>
+    <t>S8 EEE</t>
+  </si>
+  <si>
+    <t>VISHNU</t>
+  </si>
+  <si>
+    <t>SANJEEV S</t>
+  </si>
+  <si>
+    <t>SHYAMRAJ K R</t>
+  </si>
+  <si>
+    <t>KANNADEEPU MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibin Xavier                                             </t>
+  </si>
+  <si>
+    <t>SECOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senusam Biju                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jayakrishnan P                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amal V.S  </t>
+  </si>
+  <si>
+    <t>Mohammed Nihal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devanand J                                               </t>
+  </si>
+  <si>
+    <t>THIRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freddy M Thomas                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anoop Chandran B                                       </t>
+  </si>
+  <si>
+    <r>
+      <t>Ananthakrishnan G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">	</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">                 </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Jean George JoY </t>
+  </si>
+  <si>
+    <t>Meenu</t>
+  </si>
+  <si>
+    <t>Anamika</t>
+  </si>
+  <si>
+    <t>Sreelekshmi Varma</t>
+  </si>
+  <si>
+    <t>Nesla</t>
+  </si>
+  <si>
+    <t>Nayana Raj</t>
+  </si>
+  <si>
+    <t>Megha</t>
+  </si>
+  <si>
+    <t>ANJALY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> S4 CE</t>
+  </si>
+  <si>
+    <t>AKLEEMA M JAVED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> S2 CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANUSREE </t>
+  </si>
+  <si>
+    <t>SONA SASIKUMAR</t>
+  </si>
+  <si>
+    <t>ACHU RACHEL BABU</t>
+  </si>
+  <si>
+    <t>CARROMS</t>
+  </si>
+  <si>
+    <t>ANUSREE MS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,7 +690,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -571,36 +731,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -611,6 +749,14 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -654,7 +800,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -662,15 +808,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,6 +843,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -708,19 +867,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,7 +885,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,19 +933,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -786,19 +999,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -816,79 +1035,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,26 +1113,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -993,6 +1137,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1008,22 +1161,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1051,12 +1199,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1065,143 +1224,143 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1255,6 +1414,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1575,13 +1758,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:E221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="I147" sqref="I147"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H217" sqref="H217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.2222222222222" customWidth="1"/>
     <col min="2" max="2" width="16.5555555555556" customWidth="1"/>
@@ -3689,6 +3872,1124 @@
         <v>123</v>
       </c>
     </row>
+    <row r="142" spans="2:5">
+      <c r="B142" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C142" t="s">
+        <v>5</v>
+      </c>
+      <c r="D142" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E142" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5">
+      <c r="B143" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C143" t="s">
+        <v>151</v>
+      </c>
+      <c r="D143" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5">
+      <c r="B144" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C144" t="s">
+        <v>12</v>
+      </c>
+      <c r="D144" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E144" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5">
+      <c r="B145" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C145" t="s">
+        <v>17</v>
+      </c>
+      <c r="D145" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5">
+      <c r="B146" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C146" t="s">
+        <v>19</v>
+      </c>
+      <c r="D146" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5">
+      <c r="B147" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C147" t="s">
+        <v>12</v>
+      </c>
+      <c r="D147" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="148" ht="15.6" spans="2:5">
+      <c r="B148" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C148" t="s">
+        <v>10</v>
+      </c>
+      <c r="D148" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E148" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="149" ht="15.6" spans="2:5">
+      <c r="B149" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C149" t="s">
+        <v>12</v>
+      </c>
+      <c r="D149" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E149" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="150" ht="15.6" spans="2:5">
+      <c r="B150" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C150" t="s">
+        <v>5</v>
+      </c>
+      <c r="D150" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E150" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="151" ht="15.6" spans="2:5">
+      <c r="B151" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C151" t="s">
+        <v>30</v>
+      </c>
+      <c r="D151" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E151" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="152" ht="15.6" spans="2:5">
+      <c r="B152" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C152" t="s">
+        <v>12</v>
+      </c>
+      <c r="D152" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E152" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="153" ht="15.6" spans="2:5">
+      <c r="B153" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C153" t="s">
+        <v>63</v>
+      </c>
+      <c r="D153" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E153" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="154" ht="15.6" spans="2:5">
+      <c r="B154" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C154" t="s">
+        <v>32</v>
+      </c>
+      <c r="D154" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E154" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="155" ht="15.6" spans="2:5">
+      <c r="B155" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C155" t="s">
+        <v>8</v>
+      </c>
+      <c r="D155" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E155" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="156" ht="15.6" spans="2:5">
+      <c r="B156" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C156" t="s">
+        <v>30</v>
+      </c>
+      <c r="D156" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E156" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="157" ht="15.6" spans="2:5">
+      <c r="B157" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C157" t="s">
+        <v>17</v>
+      </c>
+      <c r="D157" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E157" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="158" ht="15.6" spans="2:5">
+      <c r="B158" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C158" t="s">
+        <v>12</v>
+      </c>
+      <c r="D158" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E158" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="159" ht="15.6" spans="2:5">
+      <c r="B159" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C159" t="s">
+        <v>63</v>
+      </c>
+      <c r="D159" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E159" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="160" ht="15.6" spans="2:5">
+      <c r="B160" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C160" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D160" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E160" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="161" ht="15.6" spans="2:5">
+      <c r="B161" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C161" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D161" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E161" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="162" ht="15.6" spans="2:5">
+      <c r="B162" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C162" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D162" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E162" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="163" ht="15.6" spans="2:5">
+      <c r="B163" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C163" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D163" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E163" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="164" ht="15.6" spans="2:5">
+      <c r="B164" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C164" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D164" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E164" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="165" ht="31.2" spans="2:5">
+      <c r="B165" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C165" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D165" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E165" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="166" ht="31.2" spans="2:5">
+      <c r="B166" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C166" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D166" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E166" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="167" ht="31.2" spans="2:5">
+      <c r="B167" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C167" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D167" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E167" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="168" ht="15.6" spans="2:5">
+      <c r="B168" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C168" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D168" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="169" ht="31.2" spans="2:5">
+      <c r="B169" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C169" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D169" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E169" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="170" ht="15.6" spans="2:5">
+      <c r="B170" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C170" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D170" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E170" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="171" ht="31.2" spans="2:5">
+      <c r="B171" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C171" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D171" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E171" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="172" ht="15.6" spans="2:5">
+      <c r="B172" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C172" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D172" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="173" ht="15.6" spans="2:5">
+      <c r="B173" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C173" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D173" t="s">
+        <v>6</v>
+      </c>
+      <c r="E173" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="174" ht="31.2" spans="2:5">
+      <c r="B174" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C174" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D174" t="s">
+        <v>6</v>
+      </c>
+      <c r="E174" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="175" ht="15.6" spans="2:5">
+      <c r="B175" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C175" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D175" t="s">
+        <v>6</v>
+      </c>
+      <c r="E175" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="176" ht="15.6" spans="2:5">
+      <c r="B176" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C176" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D176" t="s">
+        <v>6</v>
+      </c>
+      <c r="E176" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="177" ht="15.6" spans="2:5">
+      <c r="B177" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C177" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D177" t="s">
+        <v>6</v>
+      </c>
+      <c r="E177" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="178" ht="15.6" spans="2:5">
+      <c r="B178" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C178" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D178" t="s">
+        <v>123</v>
+      </c>
+      <c r="E178" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="179" ht="15.6" spans="2:5">
+      <c r="B179" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C179" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D179" t="s">
+        <v>123</v>
+      </c>
+      <c r="E179" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="180" ht="15.6" spans="2:5">
+      <c r="B180" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C180" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D180" t="s">
+        <v>123</v>
+      </c>
+      <c r="E180" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="181" ht="15.6" spans="2:5">
+      <c r="B181" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C181" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D181" t="s">
+        <v>123</v>
+      </c>
+      <c r="E181" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="182" ht="15.6" spans="2:5">
+      <c r="B182" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C182" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D182" t="s">
+        <v>123</v>
+      </c>
+      <c r="E182" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="183" ht="15.6" spans="2:5">
+      <c r="B183" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C183" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D183" t="s">
+        <v>123</v>
+      </c>
+      <c r="E183" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="184" ht="15.6" spans="2:5">
+      <c r="B184" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C184" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D184" t="s">
+        <v>123</v>
+      </c>
+      <c r="E184" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="185" ht="15.6" spans="2:5">
+      <c r="B185" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C185" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D185" t="s">
+        <v>123</v>
+      </c>
+      <c r="E185" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="186" ht="15.6" spans="2:5">
+      <c r="B186" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C186" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D186" t="s">
+        <v>123</v>
+      </c>
+      <c r="E186" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="187" ht="15.6" spans="2:5">
+      <c r="B187" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C187" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D187" t="s">
+        <v>123</v>
+      </c>
+      <c r="E187" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="188" ht="15.6" spans="2:5">
+      <c r="B188" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C188" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D188" t="s">
+        <v>123</v>
+      </c>
+      <c r="E188" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="189" ht="15.6" spans="2:5">
+      <c r="B189" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C189" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D189" t="s">
+        <v>123</v>
+      </c>
+      <c r="E189" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="190" ht="15.6" spans="2:5">
+      <c r="B190" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C190" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D190" t="s">
+        <v>123</v>
+      </c>
+      <c r="E190" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="191" ht="15.6" spans="2:5">
+      <c r="B191" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C191" s="23"/>
+      <c r="D191" t="s">
+        <v>123</v>
+      </c>
+      <c r="E191" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="192" ht="15.6" spans="2:5">
+      <c r="B192" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C192" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D192" t="s">
+        <v>123</v>
+      </c>
+      <c r="E192" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="193" ht="15.6" spans="2:5">
+      <c r="B193" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C193" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D193" t="s">
+        <v>123</v>
+      </c>
+      <c r="E193" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="194" ht="15.6" spans="2:5">
+      <c r="B194" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C194" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D194" t="s">
+        <v>123</v>
+      </c>
+      <c r="E194" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="195" ht="15.6" spans="2:5">
+      <c r="B195" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C195" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D195" t="s">
+        <v>123</v>
+      </c>
+      <c r="E195" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="196" ht="15.6" spans="2:5">
+      <c r="B196" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C196" t="s">
+        <v>175</v>
+      </c>
+      <c r="D196" t="s">
+        <v>123</v>
+      </c>
+      <c r="E196" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="197" ht="15.6" spans="2:5">
+      <c r="B197" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="C197" t="s">
+        <v>177</v>
+      </c>
+      <c r="D197" t="s">
+        <v>123</v>
+      </c>
+      <c r="E197" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="198" ht="15.6" spans="2:5">
+      <c r="B198" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C198" t="s">
+        <v>28</v>
+      </c>
+      <c r="D198" t="s">
+        <v>123</v>
+      </c>
+      <c r="E198" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="199" ht="15.6" spans="2:5">
+      <c r="B199" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C199" t="s">
+        <v>32</v>
+      </c>
+      <c r="D199" t="s">
+        <v>123</v>
+      </c>
+      <c r="E199" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="200" ht="15.6" spans="2:5">
+      <c r="B200" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="C200" t="s">
+        <v>32</v>
+      </c>
+      <c r="D200" t="s">
+        <v>123</v>
+      </c>
+      <c r="E200" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="201" ht="15.6" spans="2:5">
+      <c r="B201" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C201" t="s">
+        <v>28</v>
+      </c>
+      <c r="D201" t="s">
+        <v>123</v>
+      </c>
+      <c r="E201" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="202" ht="15.6" spans="2:5">
+      <c r="B202" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C202" t="s">
+        <v>28</v>
+      </c>
+      <c r="D202" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E202" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="203" ht="15.6" spans="2:5">
+      <c r="B203" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C203" t="s">
+        <v>28</v>
+      </c>
+      <c r="D203" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E203" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="204" ht="15.6" spans="2:5">
+      <c r="B204" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C204" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D204" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E204" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="205" ht="15.6" spans="2:5">
+      <c r="B205" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C205" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D205" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E205" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="206" ht="15.6" spans="2:5">
+      <c r="B206" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C206" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D206" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E206" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="207" ht="15.6" spans="2:5">
+      <c r="B207" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C207" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D207" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E207" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="208" ht="15.6" spans="2:5">
+      <c r="B208" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C208" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D208" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E208" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="209" ht="15.6" spans="2:5">
+      <c r="B209" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C209" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D209" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E209" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="210" ht="15.6" spans="2:5">
+      <c r="B210" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C210" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D210" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E210" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="211" ht="15.6" spans="2:5">
+      <c r="B211" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C211" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D211" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E211" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="212" ht="15.6" spans="2:5">
+      <c r="B212" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C212" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D212" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E212" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="213" ht="15.6" spans="2:5">
+      <c r="B213" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C213" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D213" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E213" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="214" ht="15.6" spans="2:5">
+      <c r="B214" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C214" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D214" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E214" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="215" ht="15.6" spans="2:5">
+      <c r="B215" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C215" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D215" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E215" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="216" ht="31.2" spans="2:5">
+      <c r="B216" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C216" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D216" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E216" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="217" ht="15.6" spans="2:5">
+      <c r="B217" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C217" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D217" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E217" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="218" ht="15.6" spans="2:5">
+      <c r="B218" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C218" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D218" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E218" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="219" ht="15.6" spans="2:5">
+      <c r="B219" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C219" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D219" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E219" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="220" ht="15.6" spans="2:5">
+      <c r="B220" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C220" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D220" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E220" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="221" ht="15.6" spans="2:5">
+      <c r="B221" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C221" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D221" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E221" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
tsble tennis is added
</commit_message>
<xml_diff>
--- a/assets/assets/certificate.xlsx
+++ b/assets/assets/certificate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="260">
   <si>
     <t>SI</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">               </t>
     </r>
     <r>
@@ -487,6 +493,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">             </t>
     </r>
     <r>
@@ -501,6 +513,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">       </t>
     </r>
     <r>
@@ -847,16 +865,236 @@
       <t>Lakshmi g harikumar</t>
     </r>
   </si>
+  <si>
+    <t>Anirudh M</t>
+  </si>
+  <si>
+    <t>Vyshak K</t>
+  </si>
+  <si>
+    <t>Sethumadhavan N S</t>
+  </si>
+  <si>
+    <t>Fathih Mohammed</t>
+  </si>
+  <si>
+    <t>Athul Vinayak S M</t>
+  </si>
+  <si>
+    <t>Abhiram P</t>
+  </si>
+  <si>
+    <t>Dalvin Jaijan</t>
+  </si>
+  <si>
+    <t>Sibin Sabu</t>
+  </si>
+  <si>
+    <t>86064 48184</t>
+  </si>
+  <si>
+    <t>Amal V S</t>
+  </si>
+  <si>
+    <t>Midhun Mohan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Adarsh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A S</t>
+    </r>
+  </si>
+  <si>
+    <t>99616 90690</t>
+  </si>
+  <si>
+    <t>MITHUN MURALI</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>86068 96123</t>
+    </r>
+  </si>
+  <si>
+    <t>SREERAG</t>
+  </si>
+  <si>
+    <t>95623 71022</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>MIDHUN N A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>NAAIF M SHAFI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>HARI DARSSAN. M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>HISHAMSHA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ANANDHAKRISHNAN T A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>AKSHAY KARMA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Adithya</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>EC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>S2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Amal Madhu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Aswin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Samuel</t>
+    </r>
+  </si>
+  <si>
+    <t>Ajomon biju</t>
+  </si>
+  <si>
+    <t>75929 69978</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="\+#,##0;\-#,##0"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="\+#,##0;\-#,##0"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="\+0;\-0"/>
   </numFmts>
@@ -922,15 +1160,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -943,16 +1197,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -974,16 +1229,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -997,23 +1244,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1022,9 +1253,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1037,8 +1268,22 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1054,13 +1299,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1092,13 +1330,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,37 +1390,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1152,31 +1414,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,13 +1432,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1218,13 +1456,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1236,25 +1486,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1266,13 +1504,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1372,6 +1610,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1383,30 +1639,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1426,11 +1658,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1474,152 +1712,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1673,16 +1911,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="181" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2016,10 +2251,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G234"/>
+  <dimension ref="A1:G267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="L235" sqref="L235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -6155,16 +6390,16 @@
       <c r="C180" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D180" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E180" s="20">
+      <c r="D180" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E180" s="19">
         <v>919496174807</v>
       </c>
-      <c r="F180" s="21">
+      <c r="F180" s="20">
         <v>2</v>
       </c>
-      <c r="G180" s="21">
+      <c r="G180" s="20">
         <v>0</v>
       </c>
     </row>
@@ -6178,16 +6413,16 @@
       <c r="C181" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D181" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E181" s="22">
+      <c r="D181" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E181" s="21">
         <v>919847133127</v>
       </c>
-      <c r="F181" s="21">
+      <c r="F181" s="20">
         <v>2</v>
       </c>
-      <c r="G181" s="21">
+      <c r="G181" s="20">
         <v>0</v>
       </c>
     </row>
@@ -6201,16 +6436,16 @@
       <c r="C182" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D182" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E182" s="22">
+      <c r="D182" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E182" s="21">
         <v>919562875205</v>
       </c>
-      <c r="F182" s="21">
+      <c r="F182" s="20">
         <v>2</v>
       </c>
-      <c r="G182" s="21">
+      <c r="G182" s="20">
         <v>0</v>
       </c>
     </row>
@@ -6224,16 +6459,16 @@
       <c r="C183" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D183" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E183" s="22">
+      <c r="D183" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E183" s="21">
         <v>918606749298</v>
       </c>
-      <c r="F183" s="21">
+      <c r="F183" s="20">
         <v>2</v>
       </c>
-      <c r="G183" s="21">
+      <c r="G183" s="20">
         <v>0</v>
       </c>
     </row>
@@ -6247,16 +6482,16 @@
       <c r="C184" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D184" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E184" s="22">
+      <c r="D184" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E184" s="21">
         <v>919947663257</v>
       </c>
-      <c r="F184" s="21">
+      <c r="F184" s="20">
         <v>2</v>
       </c>
-      <c r="G184" s="21">
+      <c r="G184" s="20">
         <v>0</v>
       </c>
     </row>
@@ -6270,16 +6505,16 @@
       <c r="C185" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D185" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E185" s="22">
+      <c r="D185" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E185" s="21">
         <v>919744087257</v>
       </c>
-      <c r="F185" s="21">
+      <c r="F185" s="20">
         <v>2</v>
       </c>
-      <c r="G185" s="21">
+      <c r="G185" s="20">
         <v>0</v>
       </c>
     </row>
@@ -6885,16 +7120,16 @@
       <c r="A212">
         <v>211</v>
       </c>
-      <c r="B212" s="23" t="s">
+      <c r="B212" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="C212" s="23" t="s">
+      <c r="C212" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D212" s="24" t="s">
+      <c r="D212" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E212" s="24">
+      <c r="E212" s="23">
         <v>8590817029</v>
       </c>
       <c r="F212">
@@ -6908,16 +7143,16 @@
       <c r="A213">
         <v>212</v>
       </c>
-      <c r="B213" s="23" t="s">
+      <c r="B213" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="C213" s="23" t="s">
+      <c r="C213" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D213" s="24" t="s">
+      <c r="D213" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E213" s="24">
+      <c r="E213" s="23">
         <v>9605817028</v>
       </c>
       <c r="F213">
@@ -6931,16 +7166,16 @@
       <c r="A214">
         <v>213</v>
       </c>
-      <c r="B214" s="23" t="s">
+      <c r="B214" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="C214" s="23" t="s">
+      <c r="C214" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D214" s="24" t="s">
+      <c r="D214" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E214" s="24">
+      <c r="E214" s="23">
         <v>9871435146</v>
       </c>
       <c r="F214">
@@ -6954,16 +7189,16 @@
       <c r="A215">
         <v>214</v>
       </c>
-      <c r="B215" s="23" t="s">
+      <c r="B215" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="C215" s="23" t="s">
+      <c r="C215" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D215" s="24" t="s">
+      <c r="D215" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E215" s="24">
+      <c r="E215" s="23">
         <v>7012876954</v>
       </c>
       <c r="F215">
@@ -6977,16 +7212,16 @@
       <c r="A216">
         <v>215</v>
       </c>
-      <c r="B216" s="23" t="s">
+      <c r="B216" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="C216" s="23" t="s">
+      <c r="C216" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D216" s="24" t="s">
+      <c r="D216" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E216" s="24">
+      <c r="E216" s="23">
         <v>8089039551</v>
       </c>
       <c r="F216">
@@ -7000,16 +7235,16 @@
       <c r="A217">
         <v>216</v>
       </c>
-      <c r="B217" s="23" t="s">
+      <c r="B217" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C217" s="23" t="s">
+      <c r="C217" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="D217" s="24" t="s">
+      <c r="D217" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E217" s="24">
+      <c r="E217" s="23">
         <v>7902305635</v>
       </c>
       <c r="F217">
@@ -7023,16 +7258,16 @@
       <c r="A218">
         <v>217</v>
       </c>
-      <c r="B218" s="23" t="s">
+      <c r="B218" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C218" s="23" t="s">
+      <c r="C218" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D218" s="23" t="s">
+      <c r="D218" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="E218" s="24">
+      <c r="E218" s="23">
         <v>8593899311</v>
       </c>
       <c r="F218">
@@ -7046,16 +7281,16 @@
       <c r="A219">
         <v>218</v>
       </c>
-      <c r="B219" s="23" t="s">
+      <c r="B219" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="C219" s="23" t="s">
+      <c r="C219" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D219" s="23" t="s">
+      <c r="D219" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="E219" s="25">
+      <c r="E219" s="24">
         <v>9744554438</v>
       </c>
       <c r="F219">
@@ -7069,16 +7304,16 @@
       <c r="A220">
         <v>219</v>
       </c>
-      <c r="B220" s="23" t="s">
+      <c r="B220" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="C220" s="23" t="s">
+      <c r="C220" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D220" s="23" t="s">
+      <c r="D220" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="E220" s="25">
+      <c r="E220" s="24">
         <v>9964957091</v>
       </c>
       <c r="F220">
@@ -7092,16 +7327,16 @@
       <c r="A221">
         <v>220</v>
       </c>
-      <c r="B221" s="23" t="s">
+      <c r="B221" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="C221" s="23" t="s">
+      <c r="C221" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D221" s="23" t="s">
+      <c r="D221" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="E221" s="26">
+      <c r="E221" s="25">
         <v>7560959766</v>
       </c>
       <c r="F221">
@@ -7115,16 +7350,16 @@
       <c r="A222">
         <v>221</v>
       </c>
-      <c r="B222" s="23" t="s">
+      <c r="B222" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="C222" s="23" t="s">
+      <c r="C222" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D222" s="23" t="s">
+      <c r="D222" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="E222" s="24">
+      <c r="E222" s="23">
         <v>9495160498</v>
       </c>
       <c r="F222">
@@ -7138,16 +7373,16 @@
       <c r="A223">
         <v>222</v>
       </c>
-      <c r="B223" s="23" t="s">
+      <c r="B223" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="C223" s="23" t="s">
+      <c r="C223" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D223" s="23" t="s">
+      <c r="D223" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="E223" s="26">
+      <c r="E223" s="25">
         <v>8113846597</v>
       </c>
       <c r="F223">
@@ -7408,6 +7643,765 @@
       </c>
       <c r="G234" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235" t="s">
+        <v>229</v>
+      </c>
+      <c r="C235" t="s">
+        <v>8</v>
+      </c>
+      <c r="D235" t="s">
+        <v>55</v>
+      </c>
+      <c r="E235">
+        <v>8943449525</v>
+      </c>
+      <c r="F235">
+        <v>4</v>
+      </c>
+      <c r="G235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236" t="s">
+        <v>230</v>
+      </c>
+      <c r="C236" t="s">
+        <v>8</v>
+      </c>
+      <c r="D236" t="s">
+        <v>55</v>
+      </c>
+      <c r="E236">
+        <v>9567945899</v>
+      </c>
+      <c r="F236">
+        <v>4</v>
+      </c>
+      <c r="G236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" t="s">
+        <v>231</v>
+      </c>
+      <c r="C237" t="s">
+        <v>8</v>
+      </c>
+      <c r="D237" t="s">
+        <v>55</v>
+      </c>
+      <c r="E237">
+        <v>9961732138</v>
+      </c>
+      <c r="F237">
+        <v>4</v>
+      </c>
+      <c r="G237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" t="s">
+        <v>232</v>
+      </c>
+      <c r="C238" t="s">
+        <v>8</v>
+      </c>
+      <c r="D238" t="s">
+        <v>55</v>
+      </c>
+      <c r="E238">
+        <v>8547500275</v>
+      </c>
+      <c r="F238">
+        <v>4</v>
+      </c>
+      <c r="G238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>233</v>
+      </c>
+      <c r="C239" t="s">
+        <v>8</v>
+      </c>
+      <c r="D239" t="s">
+        <v>55</v>
+      </c>
+      <c r="E239">
+        <v>7034592048</v>
+      </c>
+      <c r="F239">
+        <v>4</v>
+      </c>
+      <c r="G239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" ht="15.15" spans="1:7">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>234</v>
+      </c>
+      <c r="C240" t="s">
+        <v>8</v>
+      </c>
+      <c r="D240" t="s">
+        <v>55</v>
+      </c>
+      <c r="E240">
+        <v>9539472384</v>
+      </c>
+      <c r="F240">
+        <v>4</v>
+      </c>
+      <c r="G240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" ht="15.15" spans="1:7">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C241" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D241" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E241" s="9">
+        <v>8848516212</v>
+      </c>
+      <c r="F241">
+        <v>4</v>
+      </c>
+      <c r="G241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" ht="15.15" spans="1:7">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C242" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D242" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E242" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="F242">
+        <v>4</v>
+      </c>
+      <c r="G242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" ht="15.15" spans="1:7">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C243" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D243" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E243" s="10">
+        <v>8921571451</v>
+      </c>
+      <c r="F243">
+        <v>4</v>
+      </c>
+      <c r="G243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" ht="15.15" spans="1:7">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C244" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D244" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E244" s="10">
+        <v>8113907228</v>
+      </c>
+      <c r="F244">
+        <v>4</v>
+      </c>
+      <c r="G244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" ht="15.15" spans="1:7">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C245" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D245" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E245" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F245">
+        <v>4</v>
+      </c>
+      <c r="G245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" ht="15.15" spans="1:7">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C246" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D246" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E246" s="9">
+        <v>8301975837</v>
+      </c>
+      <c r="F246">
+        <v>4</v>
+      </c>
+      <c r="G246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" ht="15.15" spans="1:7">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C247" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D247" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E247" s="10">
+        <v>9061769935</v>
+      </c>
+      <c r="F247">
+        <v>4</v>
+      </c>
+      <c r="G247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" ht="15.15" spans="1:7">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C248" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D248" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E248" s="10">
+        <v>9072980414</v>
+      </c>
+      <c r="F248">
+        <v>4</v>
+      </c>
+      <c r="G248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" ht="15.15" spans="1:7">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C249" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D249" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E249" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F249">
+        <v>4</v>
+      </c>
+      <c r="G249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" ht="15.15" spans="1:7">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C250" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D250" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E250" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F250">
+        <v>4</v>
+      </c>
+      <c r="G250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C251" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D251" t="s">
+        <v>55</v>
+      </c>
+      <c r="E251" s="23">
+        <v>9188324563</v>
+      </c>
+      <c r="F251">
+        <v>4</v>
+      </c>
+      <c r="G251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C252" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D252" t="s">
+        <v>55</v>
+      </c>
+      <c r="E252" s="23">
+        <v>9207995289</v>
+      </c>
+      <c r="F252">
+        <v>4</v>
+      </c>
+      <c r="G252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C253" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D253" t="s">
+        <v>55</v>
+      </c>
+      <c r="E253" s="23">
+        <v>7736124331</v>
+      </c>
+      <c r="F253">
+        <v>4</v>
+      </c>
+      <c r="G253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C254" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D254" t="s">
+        <v>55</v>
+      </c>
+      <c r="E254" s="23">
+        <v>9188504295</v>
+      </c>
+      <c r="F254">
+        <v>4</v>
+      </c>
+      <c r="G254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C255" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D255" t="s">
+        <v>55</v>
+      </c>
+      <c r="E255" s="23">
+        <v>8921531028</v>
+      </c>
+      <c r="F255">
+        <v>4</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7">
+      <c r="A256">
+        <v>255</v>
+      </c>
+      <c r="B256" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="C256" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D256" t="s">
+        <v>55</v>
+      </c>
+      <c r="E256" s="23">
+        <v>8593861069</v>
+      </c>
+      <c r="F256">
+        <v>4</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C257" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D257" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="E257" s="23">
+        <v>7306121582</v>
+      </c>
+      <c r="F257">
+        <v>4</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7">
+      <c r="A258">
+        <v>257</v>
+      </c>
+      <c r="B258" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="C258" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D258" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="E258" s="23">
+        <v>8921470483</v>
+      </c>
+      <c r="F258">
+        <v>4</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C259" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D259" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="E259" s="23">
+        <v>9072165548</v>
+      </c>
+      <c r="F259">
+        <v>4</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7">
+      <c r="A260">
+        <v>259</v>
+      </c>
+      <c r="B260" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="C260" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D260" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="E260" s="23">
+        <v>9400984870</v>
+      </c>
+      <c r="F260">
+        <v>4</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7">
+      <c r="A261">
+        <v>260</v>
+      </c>
+      <c r="B261" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C261" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D261" t="s">
+        <v>55</v>
+      </c>
+      <c r="E261" s="23">
+        <v>9188324563</v>
+      </c>
+      <c r="F261">
+        <v>4</v>
+      </c>
+      <c r="G261" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7">
+      <c r="A262">
+        <v>261</v>
+      </c>
+      <c r="B262" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C262" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D262" t="s">
+        <v>55</v>
+      </c>
+      <c r="E262" s="23">
+        <v>9207995289</v>
+      </c>
+      <c r="F262">
+        <v>4</v>
+      </c>
+      <c r="G262" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7">
+      <c r="A263">
+        <v>262</v>
+      </c>
+      <c r="B263" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C263" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D263" t="s">
+        <v>55</v>
+      </c>
+      <c r="E263" s="23">
+        <v>7736124331</v>
+      </c>
+      <c r="F263">
+        <v>4</v>
+      </c>
+      <c r="G263" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7">
+      <c r="A264">
+        <v>263</v>
+      </c>
+      <c r="B264" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C264" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D264" t="s">
+        <v>55</v>
+      </c>
+      <c r="E264" s="23">
+        <v>9188504295</v>
+      </c>
+      <c r="F264">
+        <v>4</v>
+      </c>
+      <c r="G264" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7">
+      <c r="A265">
+        <v>264</v>
+      </c>
+      <c r="B265" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C265" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D265" t="s">
+        <v>55</v>
+      </c>
+      <c r="E265" s="23">
+        <v>8921531028</v>
+      </c>
+      <c r="F265">
+        <v>4</v>
+      </c>
+      <c r="G265" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7">
+      <c r="A266">
+        <v>265</v>
+      </c>
+      <c r="B266" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="C266" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D266" t="s">
+        <v>55</v>
+      </c>
+      <c r="E266" s="23">
+        <v>8593861069</v>
+      </c>
+      <c r="F266">
+        <v>4</v>
+      </c>
+      <c r="G266" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
+      <c r="A267">
+        <v>266</v>
+      </c>
+      <c r="B267" t="s">
+        <v>258</v>
+      </c>
+      <c r="C267" t="s">
+        <v>8</v>
+      </c>
+      <c r="D267" t="s">
+        <v>55</v>
+      </c>
+      <c r="E267" t="s">
+        <v>259</v>
+      </c>
+      <c r="F267">
+        <v>0</v>
+      </c>
+      <c r="G267">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed gadha to  gadha krishnan
</commit_message>
<xml_diff>
--- a/assets/assets/certificate.xlsx
+++ b/assets/assets/certificate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="296">
   <si>
     <t>SI</t>
   </si>
@@ -682,10 +682,10 @@
     <t>+91 77365 93660</t>
   </si>
   <si>
-    <t>Gadha</t>
-  </si>
-  <si>
-    <t>+91 77367 34410</t>
+    <t>Gadha Krishnan</t>
+  </si>
+  <si>
+    <t>77367 34410</t>
   </si>
   <si>
     <t>Gopika prasad</t>
@@ -864,9 +864,6 @@
       </rPr>
       <t>Lakshmi g harikumar</t>
     </r>
-  </si>
-  <si>
-    <t>Gadha krishan</t>
   </si>
   <si>
     <t>Anirudh M</t>
@@ -1090,6 +1087,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>SAYANA</t>
     </r>
     <r>
@@ -1131,6 +1134,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>ARCHANA</t>
     </r>
     <r>
@@ -1172,6 +1181,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>99649</t>
     </r>
     <r>
@@ -1222,6 +1237,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
@@ -1260,6 +1281,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
@@ -1321,11 +1348,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="\+0;\-0"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="\+#,##0;\-#,##0"/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="\+#,##0;\-#,##0"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1389,13 +1416,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1405,7 +1425,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1419,10 +1454,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1434,17 +1500,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1459,60 +1524,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1526,8 +1538,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1559,7 +1586,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1571,7 +1676,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1583,7 +1712,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1595,43 +1742,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1643,103 +1760,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1856,7 +1883,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1865,33 +1892,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1927,6 +1928,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1954,7 +1981,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1963,143 +1993,140 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2159,7 +2186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2174,34 +2201,10 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2534,8 +2537,8 @@
   <sheetPr/>
   <dimension ref="A1:G311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
-      <selection activeCell="H306" sqref="H306"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -7144,7 +7147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" ht="29.55" spans="1:7">
+    <row r="201" ht="15.15" spans="1:7">
       <c r="A201">
         <v>200</v>
       </c>
@@ -7167,7 +7170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" ht="29.55" spans="1:7">
+    <row r="202" ht="15.15" spans="1:7">
       <c r="A202">
         <v>201</v>
       </c>
@@ -7190,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" ht="29.55" spans="1:7">
+    <row r="203" ht="15.15" spans="1:7">
       <c r="A203">
         <v>202</v>
       </c>
@@ -7213,7 +7216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" ht="29.55" spans="1:7">
+    <row r="204" ht="15.15" spans="1:7">
       <c r="A204">
         <v>203</v>
       </c>
@@ -7236,7 +7239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" ht="29.55" spans="1:7">
+    <row r="205" ht="15.15" spans="1:7">
       <c r="A205">
         <v>204</v>
       </c>
@@ -7259,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" ht="29.55" spans="1:7">
+    <row r="206" ht="15.15" spans="1:7">
       <c r="A206">
         <v>205</v>
       </c>
@@ -7788,7 +7791,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="229" ht="29.55" spans="1:7">
+    <row r="229" ht="15.15" spans="1:7">
       <c r="A229">
         <v>228</v>
       </c>
@@ -7811,7 +7814,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="230" ht="29.55" spans="1:7">
+    <row r="230" ht="15.15" spans="1:7">
       <c r="A230">
         <v>229</v>
       </c>
@@ -7834,7 +7837,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="231" ht="29.55" spans="1:7">
+    <row r="231" ht="15.15" spans="1:7">
       <c r="A231">
         <v>230</v>
       </c>
@@ -7857,7 +7860,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="232" ht="29.55" spans="1:7">
+    <row r="232" ht="15.15" spans="1:7">
       <c r="A232">
         <v>231</v>
       </c>
@@ -7880,7 +7883,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="233" ht="29.55" spans="1:7">
+    <row r="233" ht="15.15" spans="1:7">
       <c r="A233">
         <v>232</v>
       </c>
@@ -7903,12 +7906,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="234" ht="29.55" spans="1:7">
+    <row r="234" ht="15.15" spans="1:7">
       <c r="A234">
         <v>233</v>
       </c>
       <c r="B234" s="10" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="C234" s="10" t="s">
         <v>8</v>
@@ -7931,7 +7934,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C235" t="s">
         <v>8</v>
@@ -7954,7 +7957,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C236" t="s">
         <v>8</v>
@@ -7977,7 +7980,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C237" t="s">
         <v>8</v>
@@ -8000,7 +8003,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C238" t="s">
         <v>8</v>
@@ -8023,7 +8026,7 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C239" t="s">
         <v>8</v>
@@ -8046,7 +8049,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C240" t="s">
         <v>8</v>
@@ -8069,7 +8072,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C241" s="9" t="s">
         <v>8</v>
@@ -8092,7 +8095,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C242" s="10" t="s">
         <v>8</v>
@@ -8101,7 +8104,7 @@
         <v>55</v>
       </c>
       <c r="E242" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F242">
         <v>4</v>
@@ -8115,7 +8118,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C243" s="10" t="s">
         <v>8</v>
@@ -8138,7 +8141,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C244" s="10" t="s">
         <v>8</v>
@@ -8161,7 +8164,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C245" s="10" t="s">
         <v>8</v>
@@ -8170,7 +8173,7 @@
         <v>55</v>
       </c>
       <c r="E245" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F245">
         <v>4</v>
@@ -8253,7 +8256,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C249" s="10" t="s">
         <v>54</v>
@@ -8262,7 +8265,7 @@
         <v>9</v>
       </c>
       <c r="E249" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F249">
         <v>4</v>
@@ -8271,12 +8274,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" ht="15.15" spans="1:7">
       <c r="A250">
         <v>249</v>
       </c>
       <c r="B250" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C250" s="10" t="s">
         <v>54</v>
@@ -8285,7 +8288,7 @@
         <v>9</v>
       </c>
       <c r="E250" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F250">
         <v>4</v>
@@ -8299,7 +8302,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C251" s="22" t="s">
         <v>221</v>
@@ -8322,7 +8325,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C252" s="22" t="s">
         <v>221</v>
@@ -8345,7 +8348,7 @@
         <v>252</v>
       </c>
       <c r="B253" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C253" s="22" t="s">
         <v>221</v>
@@ -8368,7 +8371,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C254" s="22" t="s">
         <v>221</v>
@@ -8391,7 +8394,7 @@
         <v>254</v>
       </c>
       <c r="B255" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C255" s="22" t="s">
         <v>221</v>
@@ -8414,7 +8417,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C256" s="22" t="s">
         <v>221</v>
@@ -8437,13 +8440,13 @@
         <v>256</v>
       </c>
       <c r="B257" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C257" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="C257" s="22" t="s">
+      <c r="D257" s="22" t="s">
         <v>254</v>
-      </c>
-      <c r="D257" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="E257" s="23">
         <v>7306121582</v>
@@ -8460,10 +8463,10 @@
         <v>257</v>
       </c>
       <c r="B258" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C258" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D258" s="22" t="s">
         <v>226</v>
@@ -8483,13 +8486,13 @@
         <v>258</v>
       </c>
       <c r="B259" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C259" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D259" s="22" t="s">
         <v>254</v>
-      </c>
-      <c r="D259" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="E259" s="23">
         <v>9072165548</v>
@@ -8506,10 +8509,10 @@
         <v>259</v>
       </c>
       <c r="B260" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C260" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D260" s="22" t="s">
         <v>226</v>
@@ -8529,7 +8532,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C261" s="22" t="s">
         <v>221</v>
@@ -8552,7 +8555,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C262" s="22" t="s">
         <v>221</v>
@@ -8575,7 +8578,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C263" s="22" t="s">
         <v>221</v>
@@ -8598,7 +8601,7 @@
         <v>263</v>
       </c>
       <c r="B264" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C264" s="22" t="s">
         <v>221</v>
@@ -8621,7 +8624,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C265" s="22" t="s">
         <v>221</v>
@@ -8644,7 +8647,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C266" s="22" t="s">
         <v>221</v>
@@ -8667,7 +8670,7 @@
         <v>266</v>
       </c>
       <c r="B267" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C267" t="s">
         <v>8</v>
@@ -8676,7 +8679,7 @@
         <v>55</v>
       </c>
       <c r="E267" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F267">
         <v>0</v>
@@ -8689,16 +8692,16 @@
       <c r="A268">
         <v>267</v>
       </c>
-      <c r="B268" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="C268" s="26" t="s">
+      <c r="B268" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C268" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D268" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E268" s="26">
+      <c r="D268" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E268" s="15">
         <v>8593899311</v>
       </c>
       <c r="F268">
@@ -8712,17 +8715,17 @@
       <c r="A269">
         <v>268</v>
       </c>
-      <c r="B269" s="27" t="s">
+      <c r="B269" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="C269" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D269" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E269" s="16" t="s">
         <v>262</v>
-      </c>
-      <c r="C269" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D269" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E269" s="27" t="s">
-        <v>263</v>
       </c>
       <c r="F269">
         <v>3</v>
@@ -8735,16 +8738,16 @@
       <c r="A270">
         <v>269</v>
       </c>
-      <c r="B270" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="C270" s="29" t="s">
+      <c r="B270" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C270" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="D270" s="29" t="s">
+      <c r="D270" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E270" s="30">
+      <c r="E270" s="26">
         <v>9188648541</v>
       </c>
       <c r="F270">
@@ -8758,16 +8761,16 @@
       <c r="A271">
         <v>270</v>
       </c>
-      <c r="B271" s="31" t="s">
+      <c r="B271" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C271" s="31" t="s">
+      <c r="C271" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D271" s="31" t="s">
+      <c r="D271" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E271" s="31">
+      <c r="E271" s="10">
         <v>9447347122</v>
       </c>
       <c r="F271">
@@ -8781,17 +8784,17 @@
       <c r="A272">
         <v>271</v>
       </c>
-      <c r="B272" s="31" t="s">
+      <c r="B272" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C272" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D272" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E272" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="C272" s="32" t="s">
-        <v>208</v>
-      </c>
-      <c r="D272" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E272" s="31" t="s">
-        <v>266</v>
       </c>
       <c r="F272">
         <v>3</v>
@@ -8804,17 +8807,17 @@
       <c r="A273">
         <v>272</v>
       </c>
-      <c r="B273" s="31" t="s">
+      <c r="B273" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="C273" s="32" t="s">
+      <c r="C273" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="D273" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E273" s="31" t="s">
-        <v>267</v>
+      <c r="D273" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E273" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="F273">
         <v>3</v>
@@ -8827,16 +8830,16 @@
       <c r="A274">
         <v>273</v>
       </c>
-      <c r="B274" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="C274" s="29" t="s">
+      <c r="B274" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C274" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D274" s="29" t="s">
+      <c r="D274" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E274" s="29">
+      <c r="E274" s="9">
         <v>7994474783</v>
       </c>
       <c r="F274">
@@ -8850,17 +8853,17 @@
       <c r="A275">
         <v>274</v>
       </c>
-      <c r="B275" s="31" t="s">
+      <c r="B275" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="C275" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D275" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E275" s="10" t="s">
         <v>269</v>
-      </c>
-      <c r="C275" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D275" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E275" s="31" t="s">
-        <v>270</v>
       </c>
       <c r="F275">
         <v>3</v>
@@ -8873,17 +8876,17 @@
       <c r="A276">
         <v>275</v>
       </c>
-      <c r="B276" s="31" t="s">
+      <c r="B276" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C276" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D276" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E276" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="C276" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D276" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E276" s="31" t="s">
-        <v>272</v>
       </c>
       <c r="F276">
         <v>3</v>
@@ -8896,17 +8899,17 @@
       <c r="A277">
         <v>276</v>
       </c>
-      <c r="B277" s="31" t="s">
+      <c r="B277" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C277" s="31" t="s">
+      <c r="C277" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D277" s="31" t="s">
+      <c r="D277" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E277" s="31" t="s">
-        <v>273</v>
+      <c r="E277" s="10" t="s">
+        <v>272</v>
       </c>
       <c r="F277">
         <v>3</v>
@@ -8919,17 +8922,17 @@
       <c r="A278">
         <v>277</v>
       </c>
-      <c r="B278" s="31" t="s">
+      <c r="B278" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C278" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D278" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E278" s="10" t="s">
         <v>274</v>
-      </c>
-      <c r="C278" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D278" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E278" s="31" t="s">
-        <v>275</v>
       </c>
       <c r="F278">
         <v>3</v>
@@ -8942,16 +8945,16 @@
       <c r="A279">
         <v>278</v>
       </c>
-      <c r="B279" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="C279" s="29" t="s">
+      <c r="B279" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C279" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D279" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E279" s="29">
+      <c r="D279" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E279" s="9">
         <v>9447672198</v>
       </c>
       <c r="F279">
@@ -8965,17 +8968,17 @@
       <c r="A280">
         <v>279</v>
       </c>
-      <c r="B280" s="31" t="s">
+      <c r="B280" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C280" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D280" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E280" s="10" t="s">
         <v>277</v>
-      </c>
-      <c r="C280" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D280" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E280" s="31" t="s">
-        <v>278</v>
       </c>
       <c r="F280">
         <v>3</v>
@@ -8988,16 +8991,16 @@
       <c r="A281">
         <v>280</v>
       </c>
-      <c r="B281" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="C281" s="29" t="s">
+      <c r="B281" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C281" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D281" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E281" s="29">
+      <c r="D281" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E281" s="9">
         <v>9447672198</v>
       </c>
       <c r="F281">
@@ -9011,17 +9014,17 @@
       <c r="A282">
         <v>281</v>
       </c>
-      <c r="B282" s="31" t="s">
+      <c r="B282" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C282" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D282" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E282" s="10" t="s">
         <v>277</v>
-      </c>
-      <c r="C282" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D282" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E282" s="31" t="s">
-        <v>278</v>
       </c>
       <c r="F282">
         <v>3</v>
@@ -9034,16 +9037,16 @@
       <c r="A283">
         <v>282</v>
       </c>
-      <c r="B283" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="C283" s="29" t="s">
+      <c r="B283" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C283" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="D283" s="29" t="s">
+      <c r="D283" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E283" s="30">
+      <c r="E283" s="26">
         <v>9188648541</v>
       </c>
       <c r="F283">
@@ -9057,16 +9060,16 @@
       <c r="A284">
         <v>283</v>
       </c>
-      <c r="B284" s="31" t="s">
+      <c r="B284" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C284" s="31" t="s">
+      <c r="C284" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D284" s="31" t="s">
+      <c r="D284" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E284" s="31">
+      <c r="E284" s="10">
         <v>9447347122</v>
       </c>
       <c r="F284">
@@ -9080,17 +9083,17 @@
       <c r="A285">
         <v>284</v>
       </c>
-      <c r="B285" s="31" t="s">
+      <c r="B285" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C285" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D285" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E285" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="C285" s="32" t="s">
-        <v>208</v>
-      </c>
-      <c r="D285" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E285" s="31" t="s">
-        <v>266</v>
       </c>
       <c r="F285">
         <v>3</v>
@@ -9103,17 +9106,17 @@
       <c r="A286">
         <v>285</v>
       </c>
-      <c r="B286" s="31" t="s">
+      <c r="B286" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="C286" s="32" t="s">
+      <c r="C286" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="D286" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E286" s="31" t="s">
-        <v>267</v>
+      <c r="D286" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E286" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="F286">
         <v>3</v>
@@ -9123,416 +9126,416 @@
       </c>
     </row>
     <row r="287" ht="15.15" spans="2:7">
-      <c r="B287" s="33" t="s">
+      <c r="B287" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="C287" s="33" t="s">
+      <c r="C287" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D287" s="33" t="s">
+      <c r="D287" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E287" s="37" t="s">
+      <c r="E287" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="F287" s="20">
+        <v>2</v>
+      </c>
+      <c r="G287" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" ht="15.15" spans="2:7">
+      <c r="B288" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C288" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D288" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E288" s="30" t="s">
         <v>279</v>
       </c>
-      <c r="F287" s="34">
+      <c r="F288" s="20">
         <v>2</v>
       </c>
-      <c r="G287" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" ht="15.15" spans="2:7">
-      <c r="B288" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C288" s="35" t="s">
+      <c r="G288" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" ht="15.15" spans="2:7">
+      <c r="B289" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C289" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D288" s="35" t="s">
+      <c r="D289" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E288" s="38" t="s">
+      <c r="E289" s="28">
+        <v>9562875205</v>
+      </c>
+      <c r="F289" s="20">
+        <v>2</v>
+      </c>
+      <c r="G289" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" ht="15.15" spans="2:7">
+      <c r="B290" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C290" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D290" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E290" s="28">
+        <v>8606749298</v>
+      </c>
+      <c r="F290" s="20">
+        <v>2</v>
+      </c>
+      <c r="G290" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" ht="15.15" spans="2:7">
+      <c r="B291" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C291" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D291" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E291" s="28">
+        <v>9947663257</v>
+      </c>
+      <c r="F291" s="20">
+        <v>2</v>
+      </c>
+      <c r="G291" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" ht="15.15" spans="2:7">
+      <c r="B292" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C292" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D292" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E292" s="28">
+        <v>9744087257</v>
+      </c>
+      <c r="F292" s="20">
+        <v>2</v>
+      </c>
+      <c r="G292" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" ht="15.15" spans="2:7">
+      <c r="B293" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="F288" s="34">
-        <v>2</v>
-      </c>
-      <c r="G288" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" ht="15.15" spans="2:7">
-      <c r="B289" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C289" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D289" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E289" s="36">
-        <v>9562875205</v>
-      </c>
-      <c r="F289" s="34">
-        <v>2</v>
-      </c>
-      <c r="G289" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" ht="15.15" spans="2:7">
-      <c r="B290" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="C290" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D290" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E290" s="36">
-        <v>8606749298</v>
-      </c>
-      <c r="F290" s="34">
-        <v>2</v>
-      </c>
-      <c r="G290" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" ht="15.15" spans="2:7">
-      <c r="B291" s="35" t="s">
-        <v>189</v>
-      </c>
-      <c r="C291" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D291" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E291" s="36">
-        <v>9947663257</v>
-      </c>
-      <c r="F291" s="34">
-        <v>2</v>
-      </c>
-      <c r="G291" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" ht="15.15" spans="2:7">
-      <c r="B292" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="C292" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D292" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E292" s="36">
-        <v>9744087257</v>
-      </c>
-      <c r="F292" s="34">
-        <v>2</v>
-      </c>
-      <c r="G292" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" ht="15.15" spans="2:7">
-      <c r="B293" s="26" t="s">
+      <c r="C293" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D293" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E293" s="15" t="s">
         <v>281</v>
-      </c>
-      <c r="C293" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="D293" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E293" s="26" t="s">
-        <v>282</v>
       </c>
       <c r="F293">
         <v>4</v>
       </c>
-      <c r="G293" s="34">
+      <c r="G293" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="294" ht="15.15" spans="2:7">
-      <c r="B294" s="27" t="s">
+      <c r="B294" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C294" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D294" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E294" s="16" t="s">
         <v>283</v>
-      </c>
-      <c r="C294" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="D294" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E294" s="27" t="s">
-        <v>284</v>
       </c>
       <c r="F294">
         <v>4</v>
       </c>
-      <c r="G294" s="34">
+      <c r="G294" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="295" ht="15.15" spans="2:7">
-      <c r="B295" s="27" t="s">
+      <c r="B295" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="C295" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D295" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E295" s="16" t="s">
         <v>285</v>
-      </c>
-      <c r="C295" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="D295" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E295" s="27" t="s">
-        <v>286</v>
       </c>
       <c r="F295">
         <v>4</v>
       </c>
-      <c r="G295" s="34">
+      <c r="G295" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="296" ht="15.15" spans="2:7">
-      <c r="B296" s="27" t="s">
-        <v>287</v>
-      </c>
-      <c r="C296" s="27" t="s">
+      <c r="B296" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="C296" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D296" s="27" t="s">
+      <c r="D296" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E296" s="27">
+      <c r="E296" s="16">
         <v>7306446316</v>
       </c>
       <c r="F296">
         <v>4</v>
       </c>
-      <c r="G296" s="34">
+      <c r="G296" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="297" ht="15.15" spans="2:7">
-      <c r="B297" s="27" t="s">
+      <c r="B297" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="C297" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D297" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E297" s="16" t="s">
         <v>288</v>
-      </c>
-      <c r="C297" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="D297" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E297" s="27" t="s">
-        <v>289</v>
       </c>
       <c r="F297">
         <v>4</v>
       </c>
-      <c r="G297" s="34">
+      <c r="G297" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="298" ht="15.15" spans="2:7">
-      <c r="B298" s="27" t="s">
+      <c r="B298" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="C298" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D298" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E298" s="16" t="s">
         <v>290</v>
-      </c>
-      <c r="C298" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="D298" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E298" s="27" t="s">
-        <v>291</v>
       </c>
       <c r="F298">
         <v>4</v>
       </c>
-      <c r="G298" s="34">
+      <c r="G298" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="299" ht="15.15" spans="2:7">
-      <c r="B299" s="29" t="s">
+      <c r="B299" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C299" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D299" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E299" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="C299" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D299" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E299" s="29" t="s">
-        <v>293</v>
       </c>
       <c r="F299">
         <v>4</v>
       </c>
-      <c r="G299" s="34">
+      <c r="G299" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="300" ht="15.15" spans="2:7">
-      <c r="B300" s="31" t="s">
-        <v>294</v>
-      </c>
-      <c r="C300" s="31" t="s">
+      <c r="B300" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C300" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D300" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E300" s="31" t="s">
+      <c r="D300" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E300" s="10" t="s">
         <v>155</v>
       </c>
       <c r="F300">
         <v>4</v>
       </c>
-      <c r="G300" s="34">
+      <c r="G300" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="301" ht="15.15" spans="2:7">
-      <c r="B301" s="31" t="s">
+      <c r="B301" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C301" s="31" t="s">
+      <c r="C301" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D301" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E301" s="31" t="s">
+      <c r="D301" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E301" s="10" t="s">
         <v>178</v>
       </c>
       <c r="F301">
         <v>4</v>
       </c>
-      <c r="G301" s="34">
+      <c r="G301" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="302" ht="15.15" spans="2:7">
-      <c r="B302" s="31" t="s">
+      <c r="B302" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C302" s="31" t="s">
+      <c r="C302" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D302" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E302" s="31" t="s">
+      <c r="D302" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E302" s="10" t="s">
         <v>181</v>
       </c>
       <c r="F302">
         <v>4</v>
       </c>
-      <c r="G302" s="34">
+      <c r="G302" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="303" ht="15.15" spans="2:7">
-      <c r="B303" s="29" t="s">
+      <c r="B303" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C303" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D303" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E303" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="C303" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D303" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E303" s="29" t="s">
-        <v>293</v>
       </c>
       <c r="F303">
         <v>4</v>
       </c>
-      <c r="G303" s="34" t="s">
+      <c r="G303" s="20" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="304" ht="15.15" spans="2:7">
-      <c r="B304" s="31" t="s">
+      <c r="B304" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C304" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D304" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E304" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="C304" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D304" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E304" s="31" t="s">
-        <v>295</v>
       </c>
       <c r="F304">
         <v>4</v>
       </c>
-      <c r="G304" s="34" t="s">
+      <c r="G304" s="20" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="305" ht="15.15" spans="2:7">
-      <c r="B305" s="31" t="s">
+      <c r="B305" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C305" s="31" t="s">
+      <c r="C305" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D305" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E305" s="31" t="s">
+      <c r="D305" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E305" s="10" t="s">
         <v>178</v>
       </c>
       <c r="F305">
         <v>4</v>
       </c>
-      <c r="G305" s="34" t="s">
+      <c r="G305" s="20" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="306" ht="15.15" spans="2:7">
-      <c r="B306" s="31" t="s">
+    <row r="306" spans="2:7">
+      <c r="B306" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C306" s="31" t="s">
+      <c r="C306" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D306" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E306" s="31" t="s">
+      <c r="D306" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E306" s="10" t="s">
         <v>181</v>
       </c>
       <c r="F306">
         <v>4</v>
       </c>
-      <c r="G306" s="34" t="s">
+      <c r="G306" s="20" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="307" ht="15.15" spans="2:7">
-      <c r="B307" s="29" t="s">
+      <c r="B307" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C307" s="29" t="s">
+      <c r="C307" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D307" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E307" s="29">
+      <c r="D307" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E307" s="9">
         <v>7994322927</v>
       </c>
       <c r="F307">
@@ -9543,16 +9546,16 @@
       </c>
     </row>
     <row r="308" ht="15.15" spans="2:7">
-      <c r="B308" s="31" t="s">
+      <c r="B308" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C308" s="31" t="s">
+      <c r="C308" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D308" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E308" s="31">
+      <c r="D308" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E308" s="10">
         <v>9539231717</v>
       </c>
       <c r="F308">
@@ -9563,16 +9566,16 @@
       </c>
     </row>
     <row r="309" ht="15.15" spans="2:7">
-      <c r="B309" s="31" t="s">
-        <v>296</v>
-      </c>
-      <c r="C309" s="31" t="s">
+      <c r="B309" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C309" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D309" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E309" s="31">
+      <c r="D309" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E309" s="10">
         <v>8891418626</v>
       </c>
       <c r="F309">
@@ -9583,16 +9586,16 @@
       </c>
     </row>
     <row r="310" ht="15.15" spans="2:7">
-      <c r="B310" s="31" t="s">
+      <c r="B310" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C310" s="31" t="s">
+      <c r="C310" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D310" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E310" s="31">
+      <c r="D310" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E310" s="10">
         <v>9188025758</v>
       </c>
       <c r="F310">
@@ -9602,17 +9605,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" ht="15.15" spans="2:7">
-      <c r="B311" s="31" t="s">
+    <row r="311" spans="2:7">
+      <c r="B311" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C311" s="31" t="s">
+      <c r="C311" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D311" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E311" s="31">
+      <c r="D311" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E311" s="10">
         <v>9946312522</v>
       </c>
       <c r="F311">

</xml_diff>